<commit_message>
Adjusted orientations of connectors in CPL file.
</commit_message>
<xml_diff>
--- a/470nm/CPL_JLCPCB_470nm.xlsx
+++ b/470nm/CPL_JLCPCB_470nm.xlsx
@@ -190,7 +190,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
+      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -253,7 +253,7 @@
         <v>6</v>
       </c>
       <c r="E3" s="3" t="n">
-        <v>90</v>
+        <v>270</v>
       </c>
     </row>
     <row r="4" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -270,7 +270,7 @@
         <v>6</v>
       </c>
       <c r="E4" s="3" t="n">
-        <v>270</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>